<commit_message>
fix: now you can save, update and delete students with excel file
</commit_message>
<xml_diff>
--- a/archivos/Formato Registro Estudiantes.xlsx
+++ b/archivos/Formato Registro Estudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Desktop/Universidad/Proyecto Integrador/PI1/icesi-filantrop-a-equipo-2/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E7533D-B61E-A14E-9530-02E303E32122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC196C93-2A3A-914C-96B6-40290DC2E888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="3280" windowWidth="17480" windowHeight="14960" xr2:uid="{4AB53052-041A-554A-90C9-48D2A5716275}"/>
+    <workbookView xWindow="4920" yWindow="10640" windowWidth="28680" windowHeight="9120" xr2:uid="{4AB53052-041A-554A-90C9-48D2A5716275}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>tipo_documento</t>
   </si>
@@ -77,85 +77,169 @@
     <t>CC</t>
   </si>
   <si>
-    <t>Juan Pérez</t>
-  </si>
-  <si>
-    <t>jperez@gmail.com</t>
-  </si>
-  <si>
-    <t>jperez@institucion.edu</t>
-  </si>
-  <si>
-    <t>Maria Rodriguez</t>
-  </si>
-  <si>
-    <t>mrodriguez@gmail.com</t>
-  </si>
-  <si>
-    <t>mrodriguez@institucion.edu</t>
-  </si>
-  <si>
-    <t>MR002</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
-    <t>Jane Doe</t>
-  </si>
-  <si>
-    <t>jdoe@gmail.com</t>
-  </si>
-  <si>
-    <t>jdoe@institucion.edu</t>
-  </si>
-  <si>
-    <t>JD003</t>
-  </si>
-  <si>
-    <t>Pedro Gomez</t>
-  </si>
-  <si>
-    <t>pgomez@gmail.com</t>
-  </si>
-  <si>
-    <t>pgomez@institucion.edu</t>
-  </si>
-  <si>
-    <t>PG004</t>
-  </si>
-  <si>
-    <t>A00156800</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>Andrés</t>
-  </si>
-  <si>
-    <t>andres@gmail.com</t>
-  </si>
-  <si>
     <t>4.2</t>
   </si>
   <si>
-    <t>A00123300</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
     <t>3.9</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>A00123456</t>
+  </si>
+  <si>
+    <t>4.9</t>
+  </si>
+  <si>
+    <t>A00432109</t>
+  </si>
+  <si>
+    <t>Ricardo Vargas</t>
+  </si>
+  <si>
+    <t>rvargas@gmail.com</t>
+  </si>
+  <si>
+    <t>rvargas@institucion.edu</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>A00876543</t>
+  </si>
+  <si>
+    <t>Patricia Mendoza</t>
+  </si>
+  <si>
+    <t>pmendoza@gmail.com</t>
+  </si>
+  <si>
+    <t>pmendoza@institucion.edu</t>
+  </si>
+  <si>
+    <t>A00567890</t>
+  </si>
+  <si>
+    <t>A00987654</t>
+  </si>
+  <si>
+    <t>Eduardo Jiménez</t>
+  </si>
+  <si>
+    <t>ejimenez@gmail.com</t>
+  </si>
+  <si>
+    <t>ejimenez@institucion.edu</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>A00234567</t>
+  </si>
+  <si>
+    <t>A00654321</t>
+  </si>
+  <si>
+    <t>Isabel Soto</t>
+  </si>
+  <si>
+    <t>isoto@gmail.com</t>
+  </si>
+  <si>
+    <t>isoto@institucion.edu</t>
+  </si>
+  <si>
+    <t>Jorge Ríos</t>
+  </si>
+  <si>
+    <t>jrios@gmail.com</t>
+  </si>
+  <si>
+    <t>jrios@institucion.edu</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>A00456789</t>
+  </si>
+  <si>
+    <t>A00765432</t>
+  </si>
+  <si>
+    <t>Liliana Gómez</t>
+  </si>
+  <si>
+    <t>lgomez@gmail.com</t>
+  </si>
+  <si>
+    <t>lgomez@institucion.edu</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>A00198765</t>
+  </si>
+  <si>
+    <t>Felipe Torres</t>
+  </si>
+  <si>
+    <t>ftorres@gmail.com</t>
+  </si>
+  <si>
+    <t>ftorres@institucion.edu</t>
+  </si>
+  <si>
+    <t>A00345678</t>
+  </si>
+  <si>
+    <t>Diana García</t>
+  </si>
+  <si>
+    <t>dgarcia@gmail.com</t>
+  </si>
+  <si>
+    <t>dgarcia@institucion.edu</t>
+  </si>
+  <si>
+    <t>Adrián Castro</t>
+  </si>
+  <si>
+    <t>acastro@gmail.com</t>
+  </si>
+  <si>
+    <t>acastro@institucion.edu</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>Carmen Ramírez</t>
+  </si>
+  <si>
+    <t>cramirez@gmail.com</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>A00219876</t>
   </si>
 </sst>
 </file>
@@ -208,13 +292,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -530,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFC6B80-1155-874F-8590-F55FA02751BB}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +631,7 @@
     <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
@@ -594,197 +680,383 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
-        <v>1234567890</v>
+      <c r="B2" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>367</v>
+      </c>
+      <c r="G2" s="2">
+        <v>35311</v>
+      </c>
+      <c r="H2" s="7">
+        <v>3123456789</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2">
-        <v>409</v>
-      </c>
-      <c r="G2" s="2">
-        <v>36526</v>
-      </c>
-      <c r="H2">
-        <v>3001234567</v>
-      </c>
-      <c r="I2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2">
-        <v>120</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>987654321</v>
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>146</v>
+      </c>
+      <c r="G3" s="2">
+        <v>32832</v>
+      </c>
+      <c r="H3" s="7">
+        <v>3009876543</v>
+      </c>
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="F3">
-        <v>123</v>
-      </c>
-      <c r="G3" s="2">
-        <v>36924</v>
-      </c>
-      <c r="H3">
-        <v>3009876543</v>
-      </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
       <c r="J3">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
         <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>212345678</v>
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F4">
-        <v>390</v>
+        <v>254</v>
       </c>
       <c r="G4" s="2">
-        <v>37318</v>
-      </c>
-      <c r="H4">
-        <v>3001357924</v>
+        <v>34165</v>
+      </c>
+      <c r="H4" s="7">
+        <v>3107654321</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J4">
-        <v>130</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>2345678901</v>
+      <c r="B5" t="s">
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>432</v>
+      </c>
+      <c r="G5" s="2">
+        <v>32183</v>
+      </c>
+      <c r="H5" s="7">
+        <v>3006543210</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5">
-        <v>123</v>
-      </c>
-      <c r="G5" s="2">
-        <v>37715</v>
-      </c>
-      <c r="H5">
-        <v>3002468135</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5">
-        <v>140</v>
-      </c>
-      <c r="K5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
-        <v>1107834925</v>
+      <c r="B6" t="s">
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6">
+        <v>489</v>
+      </c>
+      <c r="G6" s="2">
+        <v>33363</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3008765432</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>490</v>
+      </c>
+      <c r="G7" s="2">
+        <v>31758</v>
+      </c>
+      <c r="H7" s="7">
+        <v>3207282600</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7">
         <v>35</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6">
-        <v>320</v>
-      </c>
-      <c r="G6" s="2">
-        <v>38054</v>
-      </c>
-      <c r="H6">
-        <v>3207282500</v>
-      </c>
-      <c r="I6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6">
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8">
+        <v>345</v>
+      </c>
+      <c r="G8" s="2">
+        <v>34510</v>
+      </c>
+      <c r="H8" s="7">
+        <v>3002345678</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9">
+        <v>478</v>
+      </c>
+      <c r="G9" s="2">
+        <v>36161</v>
+      </c>
+      <c r="H9" s="7">
+        <v>3207654321</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10">
+        <v>287</v>
+      </c>
+      <c r="G10" s="2">
+        <v>35713</v>
+      </c>
+      <c r="H10" s="7">
+        <v>3129876543</v>
+      </c>
+      <c r="I10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11">
+        <v>234</v>
+      </c>
+      <c r="G11" s="2">
+        <v>33678</v>
+      </c>
+      <c r="H11" s="7">
+        <v>3201234567</v>
+      </c>
+      <c r="I11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11">
         <v>30</v>
       </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{6F4A4FBA-2EE0-5F47-B7A2-CD02BE7FFB52}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{435DF618-2A8D-9A44-848F-33D9E1000EF5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>